<commit_message>
Uploading CSSD Data Dictionary
</commit_message>
<xml_diff>
--- a/Data Dictionaries (Upload Here)/CSSD/CSSD_Data_Dictionary.xlsx
+++ b/Data Dictionaries (Upload Here)/CSSD/CSSD_Data_Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\opm-fs102\UserRedirections\WonderlyC\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A8FB0FA-FD05-42DC-AE6A-6BAA38387EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE559C2F-0886-415A-8F46-4026D5B713F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="332" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,9 +61,6 @@
     <t>Years Available</t>
   </si>
   <si>
-    <t>Judicial Branch - CSSD</t>
-  </si>
-  <si>
     <t>Bail Services</t>
   </si>
   <si>
@@ -350,6 +347,9 @@
   </si>
   <si>
     <t>Flag if there was no service recommendation</t>
+  </si>
+  <si>
+    <t>Judicial Branch - Court Support Services Division (JB-CSSD)</t>
   </si>
 </sst>
 </file>
@@ -789,7 +789,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1:H1048576"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -858,945 +858,945 @@
     </row>
     <row r="2" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>8</v>
       </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>8</v>
       </c>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>8</v>
       </c>
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" t="s">
         <v>7</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>8</v>
       </c>
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15" t="s">
         <v>7</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>8</v>
       </c>
-      <c r="C15" t="s">
-        <v>9</v>
-      </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" t="s">
         <v>7</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>8</v>
       </c>
-      <c r="C16" t="s">
-        <v>9</v>
-      </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" t="s">
         <v>7</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>8</v>
       </c>
-      <c r="C17" t="s">
-        <v>9</v>
-      </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18" t="s">
         <v>7</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>8</v>
       </c>
-      <c r="C18" t="s">
-        <v>9</v>
-      </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="B31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="B32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="B33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="B34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="B36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="B37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="B38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="B39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="B40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D40" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="B41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D41" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="B42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C42" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F42" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>